<commit_message>
Excel skjal og skýrsla eða eitthvað
</commit_message>
<xml_diff>
--- a/stadavika3.xlsx
+++ b/stadavika3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
   <si>
     <t>Validator á input</t>
   </si>
@@ -281,18 +281,6 @@
     <t>Notandi vill geta reiknað út hvaða leið er best til að borga lánin sín</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Tími unninn</t>
   </si>
   <si>
@@ -317,21 +305,9 @@
     <t>Einingapróf</t>
   </si>
   <si>
-    <t>Notendasögur færðar í næstu Ítrun</t>
-  </si>
-  <si>
     <t>Ítrun 3 (Inniheldur aðeins frestaðar notendasögur)</t>
   </si>
   <si>
-    <t>Notandi vill eta séð hve lengi hann er að safna ákveðinni upphæð      (Úr ítrun 2 í 3)</t>
-  </si>
-  <si>
-    <t>Notandi vill geta séð hagnaðinn á því að leggja fyrir                                      (Úr ítrun 2 í 3)</t>
-  </si>
-  <si>
-    <t>Notandi vill geta séð niðurstöður myndrænt                                                        (Úr ítrun 2 í 3)</t>
-  </si>
-  <si>
     <t>Heldur utan um reikninga og föll til að reikna með reikninga.</t>
   </si>
   <si>
@@ -342,6 +318,15 @@
   </si>
   <si>
     <t>Einingaprófunin fyrir ítrun 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notandi vill geta séð niðurstöður myndrænt                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notandi vill geta séð hagnaðinn á því að leggja fyrir                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notandi vill geta séð hve lengi hann er að safna ákveðinni upphæð  </t>
   </si>
 </sst>
 </file>
@@ -661,49 +646,49 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5580</c:v>
+                  <c:v>5040</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5181.4285714285716</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4782.8571428571431</c:v>
+                  <c:v>4560</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4384.2857142857147</c:v>
+                  <c:v>4320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3985.7142857142862</c:v>
+                  <c:v>4080</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3587.1428571428578</c:v>
+                  <c:v>3840</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3188.5714285714294</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2790.0000000000009</c:v>
+                  <c:v>3360</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2391.4285714285725</c:v>
+                  <c:v>3120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1992.857142857144</c:v>
+                  <c:v>2880</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1594.2857142857156</c:v>
+                  <c:v>2640</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1195.7142857142871</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>797.14285714285859</c:v>
+                  <c:v>2160</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>398.57142857143003</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1680</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,60 +764,60 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5580</c:v>
+                  <c:v>5040</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5580</c:v>
+                  <c:v>5040</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5460</c:v>
+                  <c:v>4740</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5460</c:v>
+                  <c:v>4740</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4830</c:v>
+                  <c:v>3960</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4110</c:v>
+                  <c:v>3210</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3630</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3630</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3630</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3630</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3630</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3130</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2330</c:v>
+                  <c:v>1420</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1310</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1310</c:v>
+                  <c:v>720</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="132398464"/>
-        <c:axId val="134468736"/>
+        <c:axId val="61494400"/>
+        <c:axId val="61495936"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="132398464"/>
+        <c:axId val="61494400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,14 +825,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134468736"/>
+        <c:crossAx val="61495936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="134468736"/>
+        <c:axId val="61495936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +846,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="132398464"/>
+        <c:crossAx val="61494400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,7 +898,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -989,7 +974,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$G$21:$G$28</c:f>
+              <c:f>Notendasögur!$G$40:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1065,7 +1050,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$H$22:$H$29</c:f>
+              <c:f>Notendasögur!$H$41:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1098,11 +1083,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133703168"/>
-        <c:axId val="133704704"/>
+        <c:axId val="61525376"/>
+        <c:axId val="64500864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133703168"/>
+        <c:axId val="61525376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,14 +1095,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133704704"/>
+        <c:crossAx val="64500864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133704704"/>
+        <c:axId val="64500864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1116,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="133703168"/>
+        <c:crossAx val="61525376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,7 +1168,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1226,7 +1211,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Notendasögur!$J$21:$J$28</c:f>
+              <c:f>Notendasögur!$J$40:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1259,7 +1244,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$G$40:$G$46</c:f>
+              <c:f>Notendasögur!$G$57:$G$63</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1299,7 +1284,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Notendasögur!$J$21:$J$28</c:f>
+              <c:f>Notendasögur!$J$40:$J$47</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1332,7 +1317,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$H$41:$H$47</c:f>
+              <c:f>Notendasögur!$H$58:$H$64</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1362,11 +1347,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="133721472"/>
-        <c:axId val="133739648"/>
+        <c:axId val="64525824"/>
+        <c:axId val="64527360"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="133721472"/>
+        <c:axId val="64525824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,14 +1359,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133739648"/>
+        <c:crossAx val="64527360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="133739648"/>
+        <c:axId val="64527360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1395,7 +1380,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="133721472"/>
+        <c:crossAx val="64525824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1447,7 +1432,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1494,7 +1479,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Notendasögur!$J$55:$J$61</c:f>
+              <c:f>Notendasögur!$J$72:$J$78</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1524,7 +1509,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$G$55:$G$61</c:f>
+              <c:f>Notendasögur!$G$72:$G$78</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1564,7 +1549,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Notendasögur!$J$55:$J$61</c:f>
+              <c:f>Notendasögur!$J$72:$J$78</c:f>
               <c:numCache>
                 <c:formatCode>d/m/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1594,7 +1579,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Notendasögur!$H$56:$H$62</c:f>
+              <c:f>Notendasögur!$H$73:$H$79</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1614,7 +1599,7 @@
                   <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1624,11 +1609,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="143396864"/>
-        <c:axId val="143398400"/>
+        <c:axId val="64544128"/>
+        <c:axId val="64640128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="143396864"/>
+        <c:axId val="64544128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,14 +1621,14 @@
         <c:numFmt formatCode="d/m/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143398400"/>
+        <c:crossAx val="64640128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="143398400"/>
+        <c:axId val="64640128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1642,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="143396864"/>
+        <c:crossAx val="64544128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1709,7 +1694,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1750,15 +1735,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1780,15 +1765,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>29482</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1360</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>17235</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1810,14 +1795,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>593889</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>22389</xdr:colOff>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2137,10 +2122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2180,7 +2165,7 @@
         <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
@@ -2189,11 +2174,11 @@
     <row r="2" spans="1:10">
       <c r="G2" s="6">
         <f>C65</f>
-        <v>5580</v>
+        <v>5040</v>
       </c>
       <c r="H2" s="6">
         <f>G2</f>
-        <v>5580</v>
+        <v>5040</v>
       </c>
       <c r="I2" s="6">
         <v>0</v>
@@ -2217,12 +2202,12 @@
         <v>50</v>
       </c>
       <c r="G3" s="6">
-        <f>G2-G19</f>
-        <v>5181.4285714285716</v>
+        <f>G2-G31</f>
+        <v>4800</v>
       </c>
       <c r="H3" s="6">
         <f>H2-I3</f>
-        <v>5580</v>
+        <v>5040</v>
       </c>
       <c r="I3" s="6">
         <v>0</v>
@@ -2247,12 +2232,12 @@
         <v>59</v>
       </c>
       <c r="G4" s="6">
-        <f>G3-G19</f>
-        <v>4782.8571428571431</v>
+        <f>G3-G31</f>
+        <v>4560</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H15" si="0">H3-I4</f>
-        <v>5580</v>
+        <v>5040</v>
       </c>
       <c r="I4" s="6">
         <v>0</v>
@@ -2277,15 +2262,15 @@
         <v>60</v>
       </c>
       <c r="G5" s="6">
-        <f>G4-G19</f>
-        <v>4384.2857142857147</v>
+        <f>G4-G31</f>
+        <v>4320</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>5460</v>
+        <v>4740</v>
       </c>
       <c r="I5" s="6">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="J5" s="5">
         <v>41671</v>
@@ -2307,12 +2292,12 @@
         <v>61</v>
       </c>
       <c r="G6" s="6">
-        <f>G5-G19</f>
-        <v>3985.7142857142862</v>
+        <f>G5-G31</f>
+        <v>4080</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
-        <v>5460</v>
+        <v>4740</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -2337,15 +2322,15 @@
         <v>5</v>
       </c>
       <c r="G7" s="6">
-        <f>G6-G19</f>
-        <v>3587.1428571428578</v>
+        <f>G6-G31</f>
+        <v>3840</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>4830</v>
+        <v>3960</v>
       </c>
       <c r="I7" s="6">
-        <v>630</v>
+        <v>780</v>
       </c>
       <c r="J7" s="5">
         <v>41673</v>
@@ -2355,18 +2340,18 @@
       <c r="D8" s="6"/>
       <c r="E8" s="9"/>
       <c r="F8" s="20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G8" s="6">
-        <f>G7-G19</f>
-        <v>3188.5714285714294</v>
+        <f>G7-G31</f>
+        <v>3600</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>4110</v>
+        <v>3210</v>
       </c>
       <c r="I8" s="6">
-        <v>720</v>
+        <v>750</v>
       </c>
       <c r="J8" s="5">
         <v>41674</v>
@@ -2384,18 +2369,18 @@
       <c r="D9" s="6"/>
       <c r="E9" s="9"/>
       <c r="F9" s="20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G9" s="6">
-        <f>G8-G19</f>
-        <v>2790.0000000000009</v>
+        <f>G8-G31</f>
+        <v>3360</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2400</v>
       </c>
       <c r="I9" s="6">
-        <v>480</v>
+        <v>810</v>
       </c>
       <c r="J9" s="5">
         <v>41675</v>
@@ -2413,13 +2398,16 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="9"/>
+      <c r="F10" s="20" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" s="6">
-        <f>G9-G19</f>
-        <v>2391.4285714285725</v>
+        <f>G9-G31</f>
+        <v>3120</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2400</v>
       </c>
       <c r="I10" s="6">
         <v>0</v>
@@ -2439,16 +2427,17 @@
         <v>180</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="10" t="s">
-        <v>62</v>
+      <c r="E11" s="10"/>
+      <c r="F11" s="20" t="s">
+        <v>76</v>
       </c>
       <c r="G11" s="6">
-        <f>G10-G19</f>
-        <v>1992.857142857144</v>
+        <f>G10-G31</f>
+        <v>2880</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2400</v>
       </c>
       <c r="I11" s="6">
         <v>0</v>
@@ -2468,16 +2457,17 @@
         <v>60</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="10" t="s">
-        <v>63</v>
+      <c r="E12" s="10"/>
+      <c r="F12" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="G12" s="6">
-        <f>G11-G19</f>
-        <v>1594.2857142857156</v>
+        <f>G11-G31</f>
+        <v>2640</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2400</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
@@ -2489,19 +2479,15 @@
     <row r="13" spans="1:10" ht="18.75">
       <c r="A13" s="18"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="6">
-        <f>G12-G19</f>
-        <v>1195.7142857142871</v>
+        <f>G12-G31</f>
+        <v>2400</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>3630</v>
+        <v>2400</v>
       </c>
       <c r="I13" s="6">
         <v>0</v>
@@ -2521,16 +2507,14 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="21" t="s">
-        <v>78</v>
-      </c>
+      <c r="F14" s="21"/>
       <c r="G14" s="6">
-        <f>G13-G19</f>
-        <v>797.14285714285859</v>
+        <f>G13-G31</f>
+        <v>2160</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>3130</v>
+        <v>1900</v>
       </c>
       <c r="I14" s="6">
         <v>500</v>
@@ -2551,16 +2535,14 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="21" t="s">
-        <v>77</v>
-      </c>
+      <c r="F15" s="21"/>
       <c r="G15" s="6">
-        <f>G14-G19</f>
-        <v>398.57142857143003</v>
+        <f>G14-G31</f>
+        <v>1920</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="0"/>
-        <v>2330</v>
+        <f>H14-I15 + 320</f>
+        <v>1420</v>
       </c>
       <c r="I15" s="6">
         <v>800</v>
@@ -2581,15 +2563,14 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
+      <c r="F16" s="21"/>
+      <c r="G16" s="6">
+        <f>G15-G31</f>
+        <v>1680</v>
       </c>
       <c r="H16" s="6">
-        <f>H15-I16</f>
-        <v>1310</v>
+        <f>H15-I16 + 320</f>
+        <v>720</v>
       </c>
       <c r="I16" s="6">
         <v>1020</v>
@@ -2610,11 +2591,17 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="10"/>
+      <c r="G17" s="6">
+        <f>G16-G31</f>
+        <v>1440</v>
+      </c>
       <c r="H17" s="6">
         <f>H16-I17</f>
-        <v>1310</v>
-      </c>
-      <c r="J17" s="5"/>
+        <v>720</v>
+      </c>
+      <c r="J17" s="5">
+        <v>41683</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="17">
@@ -2628,6 +2615,17 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="10"/>
+      <c r="G18" s="6">
+        <f>G17-G31</f>
+        <v>1200</v>
+      </c>
+      <c r="H18" s="6">
+        <f>H17-I18</f>
+        <v>720</v>
+      </c>
+      <c r="J18" s="5">
+        <v>41684</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="17">
@@ -2640,12 +2638,17 @@
         <v>90</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19">
-        <f>G2/14</f>
-        <v>398.57142857142856</v>
+      <c r="E19" s="11"/>
+      <c r="G19" s="6">
+        <f>G18-G31</f>
+        <v>960</v>
+      </c>
+      <c r="H19" s="6">
+        <f>H18-I19</f>
+        <v>720</v>
+      </c>
+      <c r="J19" s="5">
+        <v>41685</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2660,24 +2663,32 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="11"/>
+      <c r="G20" s="6">
+        <f>G19-G31</f>
+        <v>720</v>
+      </c>
+      <c r="H20" s="6">
+        <f>H19-I20</f>
+        <v>720</v>
+      </c>
+      <c r="J20" s="5">
+        <v>41686</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="18"/>
       <c r="D21" s="6"/>
       <c r="E21" s="11"/>
       <c r="G21" s="6">
-        <f>SUM(C3,C9,C14,C22,C27)</f>
-        <v>2640</v>
+        <f>G20-G31</f>
+        <v>480</v>
       </c>
       <c r="H21" s="6">
-        <f>G21</f>
-        <v>2640</v>
-      </c>
-      <c r="I21" s="6">
-        <v>0</v>
+        <f>H20-I21</f>
+        <v>720</v>
       </c>
       <c r="J21" s="5">
-        <v>41668</v>
+        <v>41687</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2693,17 +2704,17 @@
       <c r="E22" s="11"/>
       <c r="G22" s="6">
         <f>G21-G31</f>
-        <v>2262.8571428571427</v>
+        <v>240</v>
       </c>
       <c r="H22" s="6">
-        <f>H21-I21</f>
-        <v>2640</v>
-      </c>
-      <c r="I22" s="6">
-        <v>0</v>
+        <f>H21-I22</f>
+        <v>480</v>
+      </c>
+      <c r="I22">
+        <v>240</v>
       </c>
       <c r="J22" s="5">
-        <v>41669</v>
+        <v>41688</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2720,17 +2731,17 @@
       <c r="E23" s="3"/>
       <c r="G23" s="6">
         <f>G22-G31</f>
-        <v>1885.7142857142856</v>
+        <v>0</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" ref="H23:H29" si="1">H22-I22</f>
-        <v>2640</v>
-      </c>
-      <c r="I23" s="6">
+        <f>H22-I23</f>
         <v>0</v>
       </c>
+      <c r="I23">
+        <v>480</v>
+      </c>
       <c r="J23" s="5">
-        <v>41670</v>
+        <v>41689</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2745,20 +2756,6 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="11"/>
-      <c r="G24" s="6">
-        <f>G23-G31</f>
-        <v>1508.5714285714284</v>
-      </c>
-      <c r="H24" s="6">
-        <f t="shared" si="1"/>
-        <v>2640</v>
-      </c>
-      <c r="I24" s="6">
-        <v>300</v>
-      </c>
-      <c r="J24" s="5">
-        <v>41671</v>
-      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="17">
@@ -2772,39 +2769,11 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="11"/>
-      <c r="G25" s="6">
-        <f>G24-G31</f>
-        <v>1131.4285714285713</v>
-      </c>
-      <c r="H25" s="6">
-        <f t="shared" si="1"/>
-        <v>2340</v>
-      </c>
-      <c r="I25" s="6">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>41672</v>
-      </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="18"/>
       <c r="D26" s="6"/>
       <c r="E26" s="11"/>
-      <c r="G26" s="6">
-        <f>G25-G31</f>
-        <v>754.28571428571422</v>
-      </c>
-      <c r="H26" s="6">
-        <f t="shared" si="1"/>
-        <v>2340</v>
-      </c>
-      <c r="I26" s="6">
-        <v>780</v>
-      </c>
-      <c r="J26" s="5">
-        <v>41673</v>
-      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="17"/>
@@ -2816,20 +2785,6 @@
         <v>270</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="G27" s="6">
-        <f>G26-G31</f>
-        <v>377.14285714285705</v>
-      </c>
-      <c r="H27" s="6">
-        <f t="shared" si="1"/>
-        <v>1560</v>
-      </c>
-      <c r="I27" s="6">
-        <v>750</v>
-      </c>
-      <c r="J27" s="5">
-        <v>41674</v>
-      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="17">
@@ -2841,20 +2796,6 @@
       <c r="C28" s="13">
         <v>120</v>
       </c>
-      <c r="G28" s="6">
-        <f>G27-G31</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="6">
-        <f t="shared" si="1"/>
-        <v>810</v>
-      </c>
-      <c r="I28" s="6">
-        <v>810</v>
-      </c>
-      <c r="J28" s="5">
-        <v>41675</v>
-      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="17">
@@ -2870,10 +2811,6 @@
         <v>17</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="H29" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="17">
@@ -2889,7 +2826,6 @@
         <v>18</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="18"/>
@@ -2898,8 +2834,8 @@
       </c>
       <c r="E31" s="3"/>
       <c r="G31">
-        <f>G21/7</f>
-        <v>377.14285714285717</v>
+        <f>G2/21</f>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2991,18 +2927,18 @@
         <v>180</v>
       </c>
       <c r="G40" s="6">
-        <f>C68</f>
-        <v>2400</v>
+        <f>SUM(C3,C9,C14,C22,C27)</f>
+        <v>2640</v>
       </c>
       <c r="H40" s="6">
         <f>G40</f>
-        <v>2400</v>
-      </c>
-      <c r="I40">
+        <v>2640</v>
+      </c>
+      <c r="I40" s="6">
         <v>0</v>
       </c>
       <c r="J40" s="5">
-        <v>41676</v>
+        <v>41668</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -3016,58 +2952,58 @@
         <v>180</v>
       </c>
       <c r="G41" s="6">
-        <f>G40-G48</f>
-        <v>2000</v>
+        <f>G40-G50</f>
+        <v>2262.8571428571427</v>
       </c>
       <c r="H41" s="6">
         <f>H40-I40</f>
-        <v>2400</v>
-      </c>
-      <c r="I41">
+        <v>2640</v>
+      </c>
+      <c r="I41" s="6">
         <v>0</v>
       </c>
       <c r="J41" s="5">
-        <v>41677</v>
+        <v>41669</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="18"/>
       <c r="G42" s="6">
-        <f>G41-G48</f>
-        <v>1600</v>
+        <f>G41-G50</f>
+        <v>1885.7142857142856</v>
       </c>
       <c r="H42" s="6">
-        <f t="shared" ref="H42:H47" si="2">H41-I41</f>
-        <v>2400</v>
-      </c>
-      <c r="I42">
+        <f t="shared" ref="H42:H48" si="1">H41-I41</f>
+        <v>2640</v>
+      </c>
+      <c r="I42" s="6">
         <v>0</v>
       </c>
       <c r="J42" s="5">
-        <v>41678</v>
+        <v>41670</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="19"/>
       <c r="B43" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C43" s="15">
         <v>180</v>
       </c>
       <c r="G43" s="6">
-        <f>G42-G48</f>
-        <v>1200</v>
+        <f>G42-G50</f>
+        <v>1508.5714285714284</v>
       </c>
       <c r="H43" s="6">
-        <f t="shared" si="2"/>
-        <v>2400</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2640</v>
+      </c>
+      <c r="I43" s="6">
+        <v>300</v>
       </c>
       <c r="J43" s="5">
-        <v>41679</v>
+        <v>41671</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3075,24 +3011,24 @@
         <v>27</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C44" s="15">
         <v>120</v>
       </c>
       <c r="G44" s="6">
-        <f>G43-G48</f>
-        <v>800</v>
+        <f>G43-G50</f>
+        <v>1131.4285714285713</v>
       </c>
       <c r="H44" s="6">
-        <f t="shared" si="2"/>
-        <v>2400</v>
-      </c>
-      <c r="I44">
-        <v>500</v>
+        <f t="shared" si="1"/>
+        <v>2340</v>
+      </c>
+      <c r="I44" s="6">
+        <v>0</v>
       </c>
       <c r="J44" s="5">
-        <v>41680</v>
+        <v>41672</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -3100,52 +3036,63 @@
         <v>28</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C45" s="15">
         <v>60</v>
       </c>
       <c r="G45" s="6">
-        <f>G44-G48</f>
-        <v>400</v>
+        <f>G44-G50</f>
+        <v>754.28571428571422</v>
       </c>
       <c r="H45" s="6">
-        <f>H44-I44+320</f>
-        <v>2220</v>
-      </c>
-      <c r="I45">
-        <v>800</v>
+        <f t="shared" si="1"/>
+        <v>2340</v>
+      </c>
+      <c r="I45" s="6">
+        <v>780</v>
       </c>
       <c r="J45" s="5">
-        <v>41681</v>
+        <v>41673</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="G46" s="6">
-        <f>G45-G48</f>
-        <v>0</v>
+        <f>G45-G50</f>
+        <v>377.14285714285705</v>
       </c>
       <c r="H46" s="6">
-        <f>H45-I45+320</f>
-        <v>1740</v>
-      </c>
-      <c r="I46">
-        <v>1020</v>
+        <f t="shared" si="1"/>
+        <v>1560</v>
+      </c>
+      <c r="I46" s="6">
+        <v>750</v>
       </c>
       <c r="J46" s="5">
-        <v>41682</v>
+        <v>41674</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="14"/>
       <c r="B47" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C47" s="14">
         <v>540</v>
       </c>
+      <c r="G47" s="6">
+        <f>G46-G50</f>
+        <v>0</v>
+      </c>
       <c r="H47" s="6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>810</v>
+      </c>
+      <c r="I47" s="6">
+        <v>810</v>
+      </c>
+      <c r="J47" s="5">
+        <v>41675</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3153,14 +3100,14 @@
         <v>29</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C48" s="14">
         <v>180</v>
       </c>
-      <c r="G48">
-        <f>G40/6</f>
-        <v>400</v>
+      <c r="H48" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -3168,11 +3115,12 @@
         <v>30</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C49" s="14">
         <v>180</v>
       </c>
+      <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="19">
@@ -3184,11 +3132,15 @@
       <c r="C50" s="14">
         <v>180</v>
       </c>
+      <c r="G50">
+        <f>G40/7</f>
+        <v>377.14285714285717</v>
+      </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="14"/>
       <c r="B52" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C52" s="14">
         <v>540</v>
@@ -3208,18 +3160,6 @@
         <f>C56</f>
         <v>240</v>
       </c>
-      <c r="G55" s="6">
-        <v>720</v>
-      </c>
-      <c r="H55" s="6">
-        <v>720</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55" s="5">
-        <v>41683</v>
-      </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="22">
@@ -3231,35 +3171,21 @@
       <c r="C56" s="24">
         <v>240</v>
       </c>
-      <c r="G56" s="6">
-        <f>G55-G63</f>
-        <v>600</v>
-      </c>
-      <c r="H56" s="6">
-        <f>H55-I55</f>
-        <v>720</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56" s="5">
-        <v>41684</v>
-      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="G57" s="6">
-        <f>G56-G63</f>
-        <v>480</v>
+        <f>C68</f>
+        <v>2400</v>
       </c>
       <c r="H57" s="6">
-        <f>H56-I56</f>
-        <v>720</v>
+        <f>G57</f>
+        <v>2400</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57" s="5">
-        <v>41685</v>
+        <v>41676</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3272,18 +3198,18 @@
         <v>360</v>
       </c>
       <c r="G58" s="6">
-        <f>G57-G63</f>
-        <v>360</v>
+        <f>G57-G65</f>
+        <v>2000</v>
       </c>
       <c r="H58" s="6">
         <f>H57-I57</f>
-        <v>720</v>
+        <v>2400</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58" s="5">
-        <v>41686</v>
+        <v>41677</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3297,18 +3223,18 @@
         <v>180</v>
       </c>
       <c r="G59" s="6">
-        <f>G58-G63</f>
-        <v>240</v>
+        <f>G58-G65</f>
+        <v>1600</v>
       </c>
       <c r="H59" s="6">
-        <f>H58-I58</f>
-        <v>720</v>
+        <f t="shared" ref="H59:H61" si="2">H58-I58</f>
+        <v>2400</v>
       </c>
       <c r="I59">
         <v>0</v>
       </c>
       <c r="J59" s="5">
-        <v>41687</v>
+        <v>41678</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3322,48 +3248,58 @@
         <v>180</v>
       </c>
       <c r="G60" s="6">
-        <f>G59-G63</f>
-        <v>120</v>
+        <f>G59-G65</f>
+        <v>1200</v>
       </c>
       <c r="H60" s="6">
-        <f>H59-I59</f>
-        <v>720</v>
+        <f t="shared" si="2"/>
+        <v>2400</v>
       </c>
       <c r="I60">
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="J60" s="5">
-        <v>41688</v>
+        <v>41679</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="G61" s="6">
-        <f>G60-G63</f>
-        <v>0</v>
+        <f>G60-G65</f>
+        <v>800</v>
       </c>
       <c r="H61" s="6">
-        <f>H60-I60</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2400</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="J61" s="5">
-        <v>41689</v>
+        <v>41680</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="22"/>
       <c r="B62" s="23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C62" s="24">
         <f>C63</f>
         <v>120</v>
       </c>
+      <c r="G62" s="6">
+        <f>G61-G65</f>
+        <v>400</v>
+      </c>
       <c r="H62" s="6">
-        <f>H61-I61</f>
-        <v>0</v>
+        <f>H61-I61+320</f>
+        <v>2220</v>
+      </c>
+      <c r="I62">
+        <v>800</v>
+      </c>
+      <c r="J62" s="5">
+        <v>41681</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3371,23 +3307,42 @@
         <v>27</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C63" s="24">
         <v>120</v>
       </c>
-      <c r="G63">
-        <f>G55/6</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
+      <c r="G63" s="6">
+        <f>G62-G65</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="6">
+        <f>H62-I62+320</f>
+        <v>1740</v>
+      </c>
+      <c r="I63">
+        <v>1020</v>
+      </c>
+      <c r="J63" s="5">
+        <v>41682</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="H64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
       <c r="C65" s="6">
-        <f>SUM(C3,C9,C14,C22,C27,C32,C37,C43,C47:C52)</f>
-        <v>5580</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3">
+        <f>SUM(C3,C9,C14,C22,C27,C32,C37,C43,C47,C52)</f>
+        <v>5040</v>
+      </c>
+      <c r="G65">
+        <f>G57/6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10">
       <c r="B67" s="13" t="s">
         <v>22</v>
       </c>
@@ -3396,7 +3351,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:10">
       <c r="B68" s="14" t="s">
         <v>23</v>
       </c>
@@ -3405,13 +3360,135 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:10">
       <c r="B69" s="23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C69" s="6">
         <f>SUM(C55,C58,C62)</f>
         <v>720</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="G72" s="6">
+        <v>720</v>
+      </c>
+      <c r="H72" s="6">
+        <v>720</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72" s="5">
+        <v>41683</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="G73" s="6">
+        <f>G72-G80</f>
+        <v>600</v>
+      </c>
+      <c r="H73" s="6">
+        <f t="shared" ref="H73:H79" si="3">H72-I72</f>
+        <v>720</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73" s="5">
+        <v>41684</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="G74" s="6">
+        <f>G73-G80</f>
+        <v>480</v>
+      </c>
+      <c r="H74" s="6">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74" s="5">
+        <v>41685</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="G75" s="6">
+        <f>G74-G80</f>
+        <v>360</v>
+      </c>
+      <c r="H75" s="6">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75" s="5">
+        <v>41686</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="G76" s="6">
+        <f>G75-G80</f>
+        <v>240</v>
+      </c>
+      <c r="H76" s="6">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76" s="5">
+        <v>41687</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="G77" s="6">
+        <f>G76-G80</f>
+        <v>120</v>
+      </c>
+      <c r="H77" s="6">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="I77">
+        <v>240</v>
+      </c>
+      <c r="J77" s="5">
+        <v>41688</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="G78" s="6">
+        <f>G77-G80</f>
+        <v>0</v>
+      </c>
+      <c r="H78" s="6">
+        <f t="shared" si="3"/>
+        <v>480</v>
+      </c>
+      <c r="I78">
+        <v>480</v>
+      </c>
+      <c r="J78" s="5">
+        <v>41689</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="H79" s="6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10">
+      <c r="G80">
+        <f>G72/6</f>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3478,7 +3555,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
@@ -3510,15 +3587,15 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>